<commit_message>
verifying code for other feature
</commit_message>
<xml_diff>
--- a/com.Purchaseorder2/Testdata/Data.xlsx
+++ b/com.Purchaseorder2/Testdata/Data.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{10C18612-B25B-4AF1-B294-FEE4E0C40D09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{74F3DD48-3397-4F7E-9717-6E5644D3B2F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="20670" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20700" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Purchase" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N3"/>
+  <oleSize ref="A1:K5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -348,7 +348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -376,7 +376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38057375-291B-4893-A052-B4DC44EF1AE1}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>